<commit_message>
importaciones pendientes de resultados
</commit_message>
<xml_diff>
--- a/backend/app/templates/club_template.xlsx
+++ b/backend/app/templates/club_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joanat/Desktop/Rue/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joanat/Desktop/Rue/Templates excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4561BBDE-9407-004F-AC11-A0AFF8E04E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA91924-433A-F648-AF2C-3CECC0B292A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17980" yWindow="9000" windowWidth="28040" windowHeight="17440" xr2:uid="{7CF6AE69-7F97-9C4A-9983-551424278E18}"/>
+    <workbookView xWindow="9140" yWindow="13540" windowWidth="38900" windowHeight="18660" xr2:uid="{7CF6AE69-7F97-9C4A-9983-551424278E18}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>Persona de contacto</t>
   </si>
   <si>
-    <t>Telétono</t>
-  </si>
-  <si>
     <t>Número Club</t>
   </si>
   <si>
@@ -57,6 +54,9 @@
   </si>
   <si>
     <t>CP</t>
+  </si>
+  <si>
+    <t>Teléfono</t>
   </si>
 </sst>
 </file>
@@ -451,8 +451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{161A8729-7445-4741-943D-49D32ABD7A37}">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="136" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -470,22 +470,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>